<commit_message>
Update EPPlus 3.5 .net to 4.0. Add I18N form mono to Fix build windows platform. Testing build passed. Add UI Text to testing process.
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/Test2.xlsx
+++ b/Assets/StreamingAssets/Test2.xlsx
@@ -68,10 +68,10 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf fontId="0"/>
+    <xf numFmtId="0" fontId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf fontId="0" applyFont="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>

</xml_diff>